<commit_message>
docs: Atualizar Modificacoes em varios artefatos. Prototipo: inclui o botao Remover (PR-BR e EN-US). Ja atualizei o .fig e .pdf. Removi o .png. Editei o MCU, parte de baloes. Falta atualizar as descricoes, gerar um novo arquivo. Comecei a atualiza-las no Google Docs. Falta terminar.
</commit_message>
<xml_diff>
--- a/1.Gestão do Projeto/Gestão de Projetos - SGLV.xlsx
+++ b/1.Gestão do Projeto/Gestão de Projetos - SGLV.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFA8AEA-F1D8-443E-9DA5-B787D5784258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE1B37B-9155-49EC-BFEB-4A6552CBA492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sobre" sheetId="12" r:id="rId1"/>
@@ -1866,9 +1866,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>220980</xdr:colOff>
+          <xdr:colOff>215265</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>350520</xdr:rowOff>
+          <xdr:rowOff>358140</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2427,8 +2427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584EA1F6-5F11-49F0-BC95-54A382E64E25}">
   <dimension ref="A1:BK47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A27" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -6861,7 +6861,7 @@
         <v>40</v>
       </c>
       <c r="D25" s="108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="109">
         <v>44597</v>
@@ -7338,7 +7338,9 @@
       <c r="C27" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="108"/>
+      <c r="D27" s="108">
+        <v>1</v>
+      </c>
       <c r="E27" s="109">
         <v>44604</v>
       </c>
@@ -8049,7 +8051,9 @@
       <c r="C30" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="108"/>
+      <c r="D30" s="108">
+        <v>0</v>
+      </c>
       <c r="E30" s="109">
         <v>44611</v>
       </c>
@@ -12561,7 +12565,7 @@
       </c>
       <c r="C5" s="51">
         <f ca="1">IFERROR(IF(MIN(Marcos3[Início])=0,TODAY(),MIN(Marcos3[Início])),TODAY())</f>
-        <v>44592</v>
+        <v>44601</v>
       </c>
       <c r="E5" s="68"/>
       <c r="H5" s="39"/>
@@ -12607,7 +12611,7 @@
       <c r="N6" s="29"/>
       <c r="O6" s="29" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v/>
+        <v>março</v>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -12627,7 +12631,7 @@
       <c r="AB6" s="29"/>
       <c r="AC6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(AC7,"mmmm")=V6,TEXT(AC7,"mmmm")=O6,TEXT(AC7,"mmmm")=H6),"",TEXT(AC7,"mmmm"))</f>
-        <v>março</v>
+        <v/>
       </c>
       <c r="AD6" s="29"/>
       <c r="AE6" s="29"/>
@@ -12657,7 +12661,7 @@
       <c r="AW6" s="29"/>
       <c r="AX6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(AX7,"mmmm")=AQ6,TEXT(AX7,"mmmm")=AJ6,TEXT(AX7,"mmmm")=AC6,TEXT(AX7,"mmmm")=V6),"",TEXT(AX7,"mmmm"))</f>
-        <v/>
+        <v>abril</v>
       </c>
       <c r="AY6" s="29"/>
       <c r="AZ6" s="29"/>
@@ -12667,7 +12671,7 @@
       <c r="BD6" s="29"/>
       <c r="BE6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(BE7,"mmmm")=AX6,TEXT(BE7,"mmmm")=AQ6,TEXT(BE7,"mmmm")=AJ6,TEXT(BE7,"mmmm")=AC6),"",TEXT(BE7,"mmmm"))</f>
-        <v>abril</v>
+        <v/>
       </c>
       <c r="BF6" s="29"/>
       <c r="BG6" s="29"/>
@@ -12682,227 +12686,227 @@
       <c r="G7" s="23"/>
       <c r="H7" s="56">
         <f ca="1">IFERROR(Início_do_Projeto+Incremento_de_Rolagem,TODAY())</f>
-        <v>44605</v>
+        <v>44614</v>
       </c>
       <c r="I7" s="57">
         <f ca="1">H7+1</f>
-        <v>44606</v>
+        <v>44615</v>
       </c>
       <c r="J7" s="57">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>44607</v>
+        <v>44616</v>
       </c>
       <c r="K7" s="57">
         <f ca="1">J7+1</f>
-        <v>44608</v>
+        <v>44617</v>
       </c>
       <c r="L7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44609</v>
+        <v>44618</v>
       </c>
       <c r="M7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44610</v>
+        <v>44619</v>
       </c>
       <c r="N7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44611</v>
+        <v>44620</v>
       </c>
       <c r="O7" s="57">
         <f ca="1">N7+1</f>
-        <v>44612</v>
+        <v>44621</v>
       </c>
       <c r="P7" s="57">
         <f ca="1">O7+1</f>
-        <v>44613</v>
+        <v>44622</v>
       </c>
       <c r="Q7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44614</v>
+        <v>44623</v>
       </c>
       <c r="R7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44615</v>
+        <v>44624</v>
       </c>
       <c r="S7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44616</v>
+        <v>44625</v>
       </c>
       <c r="T7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44617</v>
+        <v>44626</v>
       </c>
       <c r="U7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44618</v>
+        <v>44627</v>
       </c>
       <c r="V7" s="57">
         <f ca="1">U7+1</f>
-        <v>44619</v>
+        <v>44628</v>
       </c>
       <c r="W7" s="57">
         <f ca="1">V7+1</f>
-        <v>44620</v>
+        <v>44629</v>
       </c>
       <c r="X7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44621</v>
+        <v>44630</v>
       </c>
       <c r="Y7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44622</v>
+        <v>44631</v>
       </c>
       <c r="Z7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44623</v>
+        <v>44632</v>
       </c>
       <c r="AA7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44624</v>
+        <v>44633</v>
       </c>
       <c r="AB7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44625</v>
+        <v>44634</v>
       </c>
       <c r="AC7" s="57">
         <f ca="1">AB7+1</f>
-        <v>44626</v>
+        <v>44635</v>
       </c>
       <c r="AD7" s="57">
         <f ca="1">AC7+1</f>
-        <v>44627</v>
+        <v>44636</v>
       </c>
       <c r="AE7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44628</v>
+        <v>44637</v>
       </c>
       <c r="AF7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44629</v>
+        <v>44638</v>
       </c>
       <c r="AG7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44630</v>
+        <v>44639</v>
       </c>
       <c r="AH7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44631</v>
+        <v>44640</v>
       </c>
       <c r="AI7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44632</v>
+        <v>44641</v>
       </c>
       <c r="AJ7" s="57">
         <f ca="1">AI7+1</f>
-        <v>44633</v>
+        <v>44642</v>
       </c>
       <c r="AK7" s="57">
         <f ca="1">AJ7+1</f>
-        <v>44634</v>
+        <v>44643</v>
       </c>
       <c r="AL7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44635</v>
+        <v>44644</v>
       </c>
       <c r="AM7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44636</v>
+        <v>44645</v>
       </c>
       <c r="AN7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44637</v>
+        <v>44646</v>
       </c>
       <c r="AO7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44638</v>
+        <v>44647</v>
       </c>
       <c r="AP7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44639</v>
+        <v>44648</v>
       </c>
       <c r="AQ7" s="57">
         <f ca="1">AP7+1</f>
-        <v>44640</v>
+        <v>44649</v>
       </c>
       <c r="AR7" s="57">
         <f ca="1">AQ7+1</f>
-        <v>44641</v>
+        <v>44650</v>
       </c>
       <c r="AS7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44642</v>
+        <v>44651</v>
       </c>
       <c r="AT7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44643</v>
+        <v>44652</v>
       </c>
       <c r="AU7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44644</v>
+        <v>44653</v>
       </c>
       <c r="AV7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44645</v>
+        <v>44654</v>
       </c>
       <c r="AW7" s="57">
         <f t="shared" ca="1" si="0"/>
-        <v>44646</v>
+        <v>44655</v>
       </c>
       <c r="AX7" s="57">
         <f ca="1">AW7+1</f>
-        <v>44647</v>
+        <v>44656</v>
       </c>
       <c r="AY7" s="57">
         <f ca="1">AX7+1</f>
-        <v>44648</v>
+        <v>44657</v>
       </c>
       <c r="AZ7" s="57">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>44649</v>
+        <v>44658</v>
       </c>
       <c r="BA7" s="57">
         <f t="shared" ca="1" si="1"/>
-        <v>44650</v>
+        <v>44659</v>
       </c>
       <c r="BB7" s="57">
         <f t="shared" ca="1" si="1"/>
-        <v>44651</v>
+        <v>44660</v>
       </c>
       <c r="BC7" s="57">
         <f t="shared" ca="1" si="1"/>
-        <v>44652</v>
+        <v>44661</v>
       </c>
       <c r="BD7" s="57">
         <f t="shared" ca="1" si="1"/>
-        <v>44653</v>
+        <v>44662</v>
       </c>
       <c r="BE7" s="57">
         <f ca="1">BD7+1</f>
-        <v>44654</v>
+        <v>44663</v>
       </c>
       <c r="BF7" s="57">
         <f ca="1">BE7+1</f>
-        <v>44655</v>
+        <v>44664</v>
       </c>
       <c r="BG7" s="57">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>44656</v>
+        <v>44665</v>
       </c>
       <c r="BH7" s="57">
         <f t="shared" ca="1" si="2"/>
-        <v>44657</v>
+        <v>44666</v>
       </c>
       <c r="BI7" s="57">
         <f t="shared" ca="1" si="2"/>
-        <v>44658</v>
+        <v>44667</v>
       </c>
       <c r="BJ7" s="57">
         <f t="shared" ca="1" si="2"/>
-        <v>44659</v>
+        <v>44668</v>
       </c>
       <c r="BK7" s="72">
         <f t="shared" ca="1" si="2"/>
-        <v>44660</v>
+        <v>44669</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -12925,27 +12929,27 @@
       <c r="G8" s="74"/>
       <c r="H8" s="58" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="I8" s="55" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="J8" s="55" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="K8" s="55" t="str">
         <f t="shared" ref="K8:BK8" ca="1" si="3">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="L8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="M8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="N8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -12953,27 +12957,27 @@
       </c>
       <c r="O8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="P8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="Q8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="R8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="S8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="T8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="U8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -12981,27 +12985,27 @@
       </c>
       <c r="V8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="W8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="X8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="Y8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="Z8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AA8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AB8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -13009,27 +13013,27 @@
       </c>
       <c r="AC8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="AD8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AE8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="AF8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AG8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AH8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AI8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -13037,27 +13041,27 @@
       </c>
       <c r="AJ8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="AK8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AL8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="AM8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AN8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AO8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AP8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -13065,27 +13069,27 @@
       </c>
       <c r="AQ8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="AR8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AS8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="AT8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AU8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AV8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AW8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -13093,27 +13097,27 @@
       </c>
       <c r="AX8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="AY8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AZ8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="BA8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BB8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BC8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BD8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -13121,27 +13125,27 @@
       </c>
       <c r="BE8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="BF8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="BG8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="BH8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BI8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BJ8" s="55" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BK8" s="73" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -13457,7 +13461,7 @@
       </c>
       <c r="E11" s="109">
         <f ca="1">TODAY()</f>
-        <v>44595</v>
+        <v>44604</v>
       </c>
       <c r="F11" s="17">
         <v>3</v>
@@ -13697,7 +13701,7 @@
       <c r="D12" s="112"/>
       <c r="E12" s="109">
         <f ca="1">TODAY()+5</f>
-        <v>44600</v>
+        <v>44609</v>
       </c>
       <c r="F12" s="17">
         <v>1</v>
@@ -13939,7 +13943,7 @@
       </c>
       <c r="E13" s="109">
         <f ca="1">TODAY()-3</f>
-        <v>44592</v>
+        <v>44601</v>
       </c>
       <c r="F13" s="17">
         <v>10</v>
@@ -14179,7 +14183,7 @@
       <c r="D14" s="112"/>
       <c r="E14" s="109">
         <f ca="1">TODAY()+20</f>
-        <v>44615</v>
+        <v>44624</v>
       </c>
       <c r="F14" s="17">
         <v>1</v>
@@ -14421,7 +14425,7 @@
       </c>
       <c r="E15" s="109">
         <f ca="1">TODAY()+6</f>
-        <v>44601</v>
+        <v>44610</v>
       </c>
       <c r="F15" s="17">
         <v>6</v>
@@ -14898,7 +14902,7 @@
       </c>
       <c r="E17" s="109">
         <f ca="1">TODAY()+6</f>
-        <v>44601</v>
+        <v>44610</v>
       </c>
       <c r="F17" s="17">
         <v>13</v>
@@ -15140,7 +15144,7 @@
       </c>
       <c r="E18" s="109">
         <f ca="1">TODAY()+7</f>
-        <v>44602</v>
+        <v>44611</v>
       </c>
       <c r="F18" s="17">
         <v>9</v>
@@ -15382,7 +15386,7 @@
       </c>
       <c r="E19" s="109">
         <f ca="1">TODAY()+15</f>
-        <v>44610</v>
+        <v>44619</v>
       </c>
       <c r="F19" s="17">
         <v>11</v>
@@ -15622,7 +15626,7 @@
       <c r="D20" s="112"/>
       <c r="E20" s="109">
         <f ca="1">TODAY()+24</f>
-        <v>44619</v>
+        <v>44628</v>
       </c>
       <c r="F20" s="17">
         <v>1</v>
@@ -15862,7 +15866,7 @@
       <c r="D21" s="111"/>
       <c r="E21" s="109">
         <f ca="1">TODAY()+25</f>
-        <v>44620</v>
+        <v>44629</v>
       </c>
       <c r="F21" s="17">
         <v>24</v>
@@ -16337,7 +16341,7 @@
       <c r="D23" s="111"/>
       <c r="E23" s="109">
         <f ca="1">TODAY()+15</f>
-        <v>44610</v>
+        <v>44619</v>
       </c>
       <c r="F23" s="17">
         <v>4</v>
@@ -16577,7 +16581,7 @@
       <c r="D24" s="112"/>
       <c r="E24" s="109">
         <f ca="1">TODAY()+19</f>
-        <v>44614</v>
+        <v>44623</v>
       </c>
       <c r="F24" s="17">
         <v>14</v>
@@ -16817,7 +16821,7 @@
       <c r="D25" s="111"/>
       <c r="E25" s="109">
         <f ca="1">TODAY()+35</f>
-        <v>44630</v>
+        <v>44639</v>
       </c>
       <c r="F25" s="17">
         <v>6</v>
@@ -17057,7 +17061,7 @@
       <c r="D26" s="112"/>
       <c r="E26" s="109">
         <f ca="1">TODAY()+48</f>
-        <v>44643</v>
+        <v>44652</v>
       </c>
       <c r="F26" s="17">
         <v>3</v>
@@ -17297,7 +17301,7 @@
       <c r="D27" s="111"/>
       <c r="E27" s="109">
         <f ca="1">TODAY()+40</f>
-        <v>44635</v>
+        <v>44644</v>
       </c>
       <c r="F27" s="17">
         <v>19</v>
@@ -17772,7 +17776,7 @@
       <c r="D29" s="111"/>
       <c r="E29" s="109">
         <f ca="1">TODAY()+37</f>
-        <v>44632</v>
+        <v>44641</v>
       </c>
       <c r="F29" s="17">
         <v>15</v>
@@ -18012,7 +18016,7 @@
       <c r="D30" s="112"/>
       <c r="E30" s="109">
         <f ca="1">TODAY()+29</f>
-        <v>44624</v>
+        <v>44633</v>
       </c>
       <c r="F30" s="17">
         <v>5</v>
@@ -18252,7 +18256,7 @@
       <c r="D31" s="111"/>
       <c r="E31" s="109">
         <f ca="1">TODAY()+80</f>
-        <v>44675</v>
+        <v>44684</v>
       </c>
       <c r="F31" s="17">
         <v>5</v>
@@ -19635,7 +19639,7 @@
       </c>
       <c r="C5" s="51">
         <f ca="1">IFERROR(IF(MIN(Marcos[Início])=0,TODAY(),MIN(Marcos[Início])),TODAY())</f>
-        <v>44592</v>
+        <v>44601</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="68"/>
@@ -19728,7 +19732,7 @@
       <c r="N6" s="29"/>
       <c r="O6" s="29" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v/>
+        <v>março</v>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -19748,7 +19752,7 @@
       <c r="AB6" s="29"/>
       <c r="AC6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(AC7,"mmmm")=V6,TEXT(AC7,"mmmm")=O6,TEXT(AC7,"mmmm")=H6),"",TEXT(AC7,"mmmm"))</f>
-        <v>março</v>
+        <v/>
       </c>
       <c r="AD6" s="29"/>
       <c r="AE6" s="29"/>
@@ -19778,7 +19782,7 @@
       <c r="AW6" s="29"/>
       <c r="AX6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(AX7,"mmmm")=AQ6,TEXT(AX7,"mmmm")=AJ6,TEXT(AX7,"mmmm")=AC6,TEXT(AX7,"mmmm")=V6),"",TEXT(AX7,"mmmm"))</f>
-        <v/>
+        <v>abril</v>
       </c>
       <c r="AY6" s="29"/>
       <c r="AZ6" s="29"/>
@@ -19788,7 +19792,7 @@
       <c r="BD6" s="29"/>
       <c r="BE6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(BE7,"mmmm")=AX6,TEXT(BE7,"mmmm")=AQ6,TEXT(BE7,"mmmm")=AJ6,TEXT(BE7,"mmmm")=AC6),"",TEXT(BE7,"mmmm"))</f>
-        <v>abril</v>
+        <v/>
       </c>
       <c r="BF6" s="29"/>
       <c r="BG6" s="29"/>
@@ -19806,227 +19810,227 @@
       <c r="G7" s="23"/>
       <c r="H7" s="59">
         <f ca="1">IFERROR(Início_do_Projeto+Incremento_de_Rolagem,TODAY())</f>
-        <v>44605</v>
+        <v>44614</v>
       </c>
       <c r="I7" s="61">
         <f ca="1">H7+1</f>
-        <v>44606</v>
+        <v>44615</v>
       </c>
       <c r="J7" s="61">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>44607</v>
+        <v>44616</v>
       </c>
       <c r="K7" s="61">
         <f ca="1">J7+1</f>
-        <v>44608</v>
+        <v>44617</v>
       </c>
       <c r="L7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44609</v>
+        <v>44618</v>
       </c>
       <c r="M7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44610</v>
+        <v>44619</v>
       </c>
       <c r="N7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44611</v>
+        <v>44620</v>
       </c>
       <c r="O7" s="61">
         <f ca="1">N7+1</f>
-        <v>44612</v>
+        <v>44621</v>
       </c>
       <c r="P7" s="61">
         <f ca="1">O7+1</f>
-        <v>44613</v>
+        <v>44622</v>
       </c>
       <c r="Q7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44614</v>
+        <v>44623</v>
       </c>
       <c r="R7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44615</v>
+        <v>44624</v>
       </c>
       <c r="S7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44616</v>
+        <v>44625</v>
       </c>
       <c r="T7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44617</v>
+        <v>44626</v>
       </c>
       <c r="U7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44618</v>
+        <v>44627</v>
       </c>
       <c r="V7" s="61">
         <f ca="1">U7+1</f>
-        <v>44619</v>
+        <v>44628</v>
       </c>
       <c r="W7" s="61">
         <f ca="1">V7+1</f>
-        <v>44620</v>
+        <v>44629</v>
       </c>
       <c r="X7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44621</v>
+        <v>44630</v>
       </c>
       <c r="Y7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44622</v>
+        <v>44631</v>
       </c>
       <c r="Z7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44623</v>
+        <v>44632</v>
       </c>
       <c r="AA7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44624</v>
+        <v>44633</v>
       </c>
       <c r="AB7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44625</v>
+        <v>44634</v>
       </c>
       <c r="AC7" s="61">
         <f ca="1">AB7+1</f>
-        <v>44626</v>
+        <v>44635</v>
       </c>
       <c r="AD7" s="61">
         <f ca="1">AC7+1</f>
-        <v>44627</v>
+        <v>44636</v>
       </c>
       <c r="AE7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44628</v>
+        <v>44637</v>
       </c>
       <c r="AF7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44629</v>
+        <v>44638</v>
       </c>
       <c r="AG7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44630</v>
+        <v>44639</v>
       </c>
       <c r="AH7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44631</v>
+        <v>44640</v>
       </c>
       <c r="AI7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44632</v>
+        <v>44641</v>
       </c>
       <c r="AJ7" s="61">
         <f ca="1">AI7+1</f>
-        <v>44633</v>
+        <v>44642</v>
       </c>
       <c r="AK7" s="61">
         <f ca="1">AJ7+1</f>
-        <v>44634</v>
+        <v>44643</v>
       </c>
       <c r="AL7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44635</v>
+        <v>44644</v>
       </c>
       <c r="AM7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44636</v>
+        <v>44645</v>
       </c>
       <c r="AN7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44637</v>
+        <v>44646</v>
       </c>
       <c r="AO7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44638</v>
+        <v>44647</v>
       </c>
       <c r="AP7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44639</v>
+        <v>44648</v>
       </c>
       <c r="AQ7" s="61">
         <f ca="1">AP7+1</f>
-        <v>44640</v>
+        <v>44649</v>
       </c>
       <c r="AR7" s="61">
         <f ca="1">AQ7+1</f>
-        <v>44641</v>
+        <v>44650</v>
       </c>
       <c r="AS7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44642</v>
+        <v>44651</v>
       </c>
       <c r="AT7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44643</v>
+        <v>44652</v>
       </c>
       <c r="AU7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44644</v>
+        <v>44653</v>
       </c>
       <c r="AV7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44645</v>
+        <v>44654</v>
       </c>
       <c r="AW7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44646</v>
+        <v>44655</v>
       </c>
       <c r="AX7" s="61">
         <f ca="1">AW7+1</f>
-        <v>44647</v>
+        <v>44656</v>
       </c>
       <c r="AY7" s="61">
         <f ca="1">AX7+1</f>
-        <v>44648</v>
+        <v>44657</v>
       </c>
       <c r="AZ7" s="61">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>44649</v>
+        <v>44658</v>
       </c>
       <c r="BA7" s="61">
         <f t="shared" ca="1" si="1"/>
-        <v>44650</v>
+        <v>44659</v>
       </c>
       <c r="BB7" s="61">
         <f t="shared" ca="1" si="1"/>
-        <v>44651</v>
+        <v>44660</v>
       </c>
       <c r="BC7" s="61">
         <f t="shared" ca="1" si="1"/>
-        <v>44652</v>
+        <v>44661</v>
       </c>
       <c r="BD7" s="61">
         <f t="shared" ca="1" si="1"/>
-        <v>44653</v>
+        <v>44662</v>
       </c>
       <c r="BE7" s="61">
         <f ca="1">BD7+1</f>
-        <v>44654</v>
+        <v>44663</v>
       </c>
       <c r="BF7" s="61">
         <f ca="1">BE7+1</f>
-        <v>44655</v>
+        <v>44664</v>
       </c>
       <c r="BG7" s="61">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>44656</v>
+        <v>44665</v>
       </c>
       <c r="BH7" s="61">
         <f t="shared" ca="1" si="2"/>
-        <v>44657</v>
+        <v>44666</v>
       </c>
       <c r="BI7" s="61">
         <f t="shared" ca="1" si="2"/>
-        <v>44658</v>
+        <v>44667</v>
       </c>
       <c r="BJ7" s="61">
         <f t="shared" ca="1" si="2"/>
-        <v>44659</v>
+        <v>44668</v>
       </c>
       <c r="BK7" s="30">
         <f t="shared" ca="1" si="2"/>
-        <v>44660</v>
+        <v>44669</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="30.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -20049,27 +20053,27 @@
       <c r="G8" s="64"/>
       <c r="H8" s="63" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="I8" s="62" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="J8" s="62" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="K8" s="62" t="str">
         <f t="shared" ref="K8:AM8" ca="1" si="3">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="L8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="M8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="N8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -20077,27 +20081,27 @@
       </c>
       <c r="O8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="P8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="Q8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="R8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="S8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="T8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="U8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -20105,27 +20109,27 @@
       </c>
       <c r="V8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="W8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="X8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="Y8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="Z8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AA8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AB8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -20133,27 +20137,27 @@
       </c>
       <c r="AC8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="AD8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AE8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="AF8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AG8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AH8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AI8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -20161,27 +20165,27 @@
       </c>
       <c r="AJ8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="AK8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AL8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="AM8" s="62" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AN8" s="62" t="str">
         <f t="shared" ref="AN8:BK8" ca="1" si="4">LEFT(TEXT(AN7,"ddd"),1)</f>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AO8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AP8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -20189,27 +20193,27 @@
       </c>
       <c r="AQ8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="AR8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AS8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="AT8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AU8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AV8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AW8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -20217,27 +20221,27 @@
       </c>
       <c r="AX8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="AY8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AZ8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="BA8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BB8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BC8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BD8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -20245,27 +20249,27 @@
       </c>
       <c r="BE8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>t</v>
       </c>
       <c r="BF8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="BG8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>q</v>
       </c>
       <c r="BH8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BI8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BJ8" s="62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BK8" s="60" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -20582,7 +20586,7 @@
       </c>
       <c r="E11" s="109">
         <f ca="1">TODAY()</f>
-        <v>44595</v>
+        <v>44604</v>
       </c>
       <c r="F11" s="17">
         <v>3</v>
@@ -20822,7 +20826,7 @@
       <c r="D12" s="113"/>
       <c r="E12" s="109">
         <f ca="1">TODAY()+5</f>
-        <v>44600</v>
+        <v>44609</v>
       </c>
       <c r="F12" s="17">
         <v>1</v>
@@ -21064,7 +21068,7 @@
       </c>
       <c r="E13" s="109">
         <f ca="1">TODAY()-3</f>
-        <v>44592</v>
+        <v>44601</v>
       </c>
       <c r="F13" s="17">
         <v>10</v>
@@ -21304,7 +21308,7 @@
       <c r="D14" s="113"/>
       <c r="E14" s="109">
         <f ca="1">TODAY()+20</f>
-        <v>44615</v>
+        <v>44624</v>
       </c>
       <c r="F14" s="17">
         <v>1</v>
@@ -21546,7 +21550,7 @@
       </c>
       <c r="E15" s="109">
         <f ca="1">TODAY()+6</f>
-        <v>44601</v>
+        <v>44610</v>
       </c>
       <c r="F15" s="17">
         <v>6</v>
@@ -22023,7 +22027,7 @@
       </c>
       <c r="E17" s="109">
         <f ca="1">TODAY()+6</f>
-        <v>44601</v>
+        <v>44610</v>
       </c>
       <c r="F17" s="17">
         <v>13</v>
@@ -22265,7 +22269,7 @@
       </c>
       <c r="E18" s="109">
         <f ca="1">TODAY()+7</f>
-        <v>44602</v>
+        <v>44611</v>
       </c>
       <c r="F18" s="17">
         <v>9</v>
@@ -22507,7 +22511,7 @@
       </c>
       <c r="E19" s="109">
         <f ca="1">TODAY()+15</f>
-        <v>44610</v>
+        <v>44619</v>
       </c>
       <c r="F19" s="17">
         <v>11</v>
@@ -22747,7 +22751,7 @@
       <c r="D20" s="113"/>
       <c r="E20" s="109">
         <f ca="1">TODAY()+24</f>
-        <v>44619</v>
+        <v>44628</v>
       </c>
       <c r="F20" s="17">
         <v>1</v>
@@ -22987,7 +22991,7 @@
       <c r="D21" s="113"/>
       <c r="E21" s="109">
         <f ca="1">TODAY()+25</f>
-        <v>44620</v>
+        <v>44629</v>
       </c>
       <c r="F21" s="17">
         <v>24</v>
@@ -23462,7 +23466,7 @@
       <c r="D23" s="113"/>
       <c r="E23" s="109">
         <f ca="1">TODAY()+15</f>
-        <v>44610</v>
+        <v>44619</v>
       </c>
       <c r="F23" s="17">
         <v>4</v>
@@ -23702,7 +23706,7 @@
       <c r="D24" s="113"/>
       <c r="E24" s="109">
         <f ca="1">TODAY()+19</f>
-        <v>44614</v>
+        <v>44623</v>
       </c>
       <c r="F24" s="17">
         <v>14</v>
@@ -23942,7 +23946,7 @@
       <c r="D25" s="113"/>
       <c r="E25" s="109">
         <f ca="1">TODAY()+35</f>
-        <v>44630</v>
+        <v>44639</v>
       </c>
       <c r="F25" s="17">
         <v>6</v>
@@ -24182,7 +24186,7 @@
       <c r="D26" s="113"/>
       <c r="E26" s="109">
         <f ca="1">TODAY()+48</f>
-        <v>44643</v>
+        <v>44652</v>
       </c>
       <c r="F26" s="17">
         <v>3</v>
@@ -24422,7 +24426,7 @@
       <c r="D27" s="113"/>
       <c r="E27" s="109">
         <f ca="1">TODAY()+40</f>
-        <v>44635</v>
+        <v>44644</v>
       </c>
       <c r="F27" s="17">
         <v>19</v>
@@ -24897,7 +24901,7 @@
       <c r="D29" s="113"/>
       <c r="E29" s="109">
         <f ca="1">TODAY()+37</f>
-        <v>44632</v>
+        <v>44641</v>
       </c>
       <c r="F29" s="17">
         <v>15</v>
@@ -25137,7 +25141,7 @@
       <c r="D30" s="113"/>
       <c r="E30" s="109">
         <f ca="1">TODAY()+29</f>
-        <v>44624</v>
+        <v>44633</v>
       </c>
       <c r="F30" s="17">
         <v>5</v>
@@ -25377,7 +25381,7 @@
       <c r="D31" s="113"/>
       <c r="E31" s="109">
         <f ca="1">TODAY()+80</f>
-        <v>44675</v>
+        <v>44684</v>
       </c>
       <c r="F31" s="17">
         <v>5</v>

</xml_diff>